<commit_message>
izmijenio primjer xlsx-a, u formi za unos racuna postavljeno da se pokazuju svi racuni na drugu decimalu, postavljeno da prepoznaju zarez kao decimalnu tocku
</commit_message>
<xml_diff>
--- a/app/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
+++ b/app/assets/Sablona_za_nenaplacena_potrazivanja_primjer-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-1880" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Zaglavlje" sheetId="1" r:id="rId1"/>
@@ -140,8 +140,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ _H_R_K"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,14 +190,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +607,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +641,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>
@@ -656,16 +659,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -679,13 +683,13 @@
       <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -702,13 +706,13 @@
       <c r="C2" s="2">
         <v>42439</v>
       </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="8">
+        <v>10000.5</v>
+      </c>
+      <c r="E2" s="8">
         <v>500</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>1500</v>
       </c>
       <c r="G2" s="3">
@@ -725,14 +729,14 @@
       <c r="C3" s="2">
         <v>42470</v>
       </c>
-      <c r="D3">
-        <v>20000</v>
-      </c>
-      <c r="E3">
-        <v>200</v>
-      </c>
-      <c r="F3">
-        <v>2000</v>
+      <c r="D3" s="8">
+        <v>20000.66</v>
+      </c>
+      <c r="E3" s="8">
+        <v>200.66</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2000.66</v>
       </c>
       <c r="G3" s="3">
         <v>29524210204</v>
@@ -748,13 +752,13 @@
       <c r="C4" s="2">
         <v>42379</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>50000</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>1500</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>3200</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -763,5 +767,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="G4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>